<commit_message>
Added perplexity and add-k smoothing
also updated the data train and test
</commit_message>
<xml_diff>
--- a/dataTrainTitle.xlsx
+++ b/dataTrainTitle.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\Agony stuff\NLP\Tugas #1 LM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>It'll Be Years Before The New 'R36' Nissan GT-R Arrives</t>
   </si>
@@ -33,6 +33,264 @@
   </si>
   <si>
     <t>The 2020 Nissan GT-R Nismo Is Almost 600LT Money</t>
+  </si>
+  <si>
+    <t>Nissan Has Put The RB26 Back Into Production</t>
+  </si>
+  <si>
+    <t>BMW Has Reportedly Already Decided Not To Replace The New Z4</t>
+  </si>
+  <si>
+    <t>ABT Has Revealed The 236bhp 'S1' That Audi Won’t Make</t>
+  </si>
+  <si>
+    <t>An All-Electric Cupra Concept Is Coming With A Funky Steering Wheel And Many LEDs</t>
+  </si>
+  <si>
+    <t>The New Audi RS6 Is Hiding 592bhp Under Its Blistered Arches</t>
+  </si>
+  <si>
+    <t>The Rodin FZed Is A Track Car That Lets You Live Out Your F1 Dreams</t>
+  </si>
+  <si>
+    <t>Lotus Evija Is A Surprisingly Lightweight Electric Hypercar With 2000bhp</t>
+  </si>
+  <si>
+    <t>Lotus Is Building An All-Electric Hypercar To Combat Rimac</t>
+  </si>
+  <si>
+    <t>Surprise: The Lincoln Aviator Hybrid Kicks Out Nearly 500bhp And Over 600lb ft</t>
+  </si>
+  <si>
+    <t>Aston Martin’s Original Vanquish Has Been Reworked For 2019</t>
+  </si>
+  <si>
+    <t>The Next Hyundai i10 Will Look Surprisingly Angry</t>
+  </si>
+  <si>
+    <t>De Tomaso Announces Its Comeback With Achingly Beautiful P72</t>
+  </si>
+  <si>
+    <t>The Bugatti Chiron Has Topped 300mph, And The Footage Is Incredible</t>
+  </si>
+  <si>
+    <t>Hennessey Will Extract 1200bhp From Your Shelby Mustang GT500</t>
+  </si>
+  <si>
+    <t>The Ford Mustang GT350R Has Been Made Faster With GT500 Stuff</t>
+  </si>
+  <si>
+    <t>The Ford GT Mk II Is A 700bhp, $1.2m Track-Only Supercar</t>
+  </si>
+  <si>
+    <t>The 2020 Mustang GT500 Will Rearrange Your Face With A 10.6s 0-100-0 Time</t>
+  </si>
+  <si>
+    <t>Mazda Will Lightly Modify Your ND MX-5 With These New Accessory Packs</t>
+  </si>
+  <si>
+    <t>Mazda Could Make A 3 Hot Hatch, But It Isn't Going To</t>
+  </si>
+  <si>
+    <t>Mazda's Clever 175bhp Petrol Engine Does 52mpg And Emits Only 96g/km</t>
+  </si>
+  <si>
+    <t>Mazda Is Building An All-New N/A Straight-Six</t>
+  </si>
+  <si>
+    <t>This Electric Open-Top Renault Is The 4L That 2019 Needs Immediately</t>
+  </si>
+  <si>
+    <t>The Mitsubishi Lancer Evo Might Be Coming Back After All</t>
+  </si>
+  <si>
+    <t>The New-Ish Renault Zoe Has A 242-Mile Range</t>
+  </si>
+  <si>
+    <t>FWD And 4-Door 'Ring Records 'Broken' By Super Saloon With Polestar Blood</t>
+  </si>
+  <si>
+    <t>The Porsche Taycan Is The 'Ring's Fastest Road-Legal EV</t>
+  </si>
+  <si>
+    <t>Jaguar’s First Mid-Engined Racer Is Reborn – And It’s Road Legal</t>
+  </si>
+  <si>
+    <t>This Might Be Lamborghini's Long-Rumoured Hypercar</t>
+  </si>
+  <si>
+    <t>Lamborghini Aventador SVJ 63 And Huracan Evo GT Arrive: Who Cares About Subtlety Anyway?</t>
+  </si>
+  <si>
+    <t>671bhp Porsche Cayenne Turbo S E-Hybrid Wades Into The SUV Power Battle</t>
+  </si>
+  <si>
+    <t>Meet The Armoured BMW X5 That Calls Itself VR6</t>
+  </si>
+  <si>
+    <t>The Vantablack-Coated BMW X6 Is A Road-Going Stealth Bomber</t>
+  </si>
+  <si>
+    <t>The New Subaru Outback Is Here To Be Quietly Brilliant Again</t>
+  </si>
+  <si>
+    <t>The Subaru WRX STI S209 Is All-But Confirmed For The USA</t>
+  </si>
+  <si>
+    <t>It Looks Like A Subaru WRX STI S209 Is Coming To The USA</t>
+  </si>
+  <si>
+    <t>Toyota, Subaru Reportedly Planning A ‘New MR2’ With Up To 300bhp</t>
+  </si>
+  <si>
+    <t>The New Mercedes-AMG '45 Range Tops Out At Nearly £60,000</t>
+  </si>
+  <si>
+    <t>Mercedes-AMG's GLB 35 Turned Out To Be A Handsome, Boxy Surprise</t>
+  </si>
+  <si>
+    <t>The Mercedes-AMG GLB 35 Is Another Way To Get Half-Fat Affalterbach Kicks</t>
+  </si>
+  <si>
+    <t>Hyundai’s Luxury Brand Genesis Is Coming For The UK In 2020</t>
+  </si>
+  <si>
+    <t>Honda’s Rear-Wheel Drive ‘E Prototype’ Electric Supermini Is Here</t>
+  </si>
+  <si>
+    <t>The All-New 600bhp Alfa Romeo GTV Has Been Leaked (Update: No It Hasn't)</t>
+  </si>
+  <si>
+    <t>F1-Inspired Alfa Romeo Racing Giulia And Stelvio Quadrifoglio Models Revealed</t>
+  </si>
+  <si>
+    <t>The Cupra Tavascan Is Another SUV From Seat's Sporty Sub-Brand</t>
+  </si>
+  <si>
+    <t>McLaren’s New 245mph Hyper-GT Will Be Named Speedtail</t>
+  </si>
+  <si>
+    <t>This Is The 1000bhp McLaren Speedtail’s Speedy Tail</t>
+  </si>
+  <si>
+    <t>The Rimac-Battling Lotus Type 130 Electric Hypercar Will Be Here In July</t>
+  </si>
+  <si>
+    <t>The Lamborghini Huracán Sterrato Is The Off-Road Supercar Of Your Dreams</t>
+  </si>
+  <si>
+    <t>Brits Can Finally Order A Right-Hand Drive Tesla Model 3</t>
+  </si>
+  <si>
+    <t>The Cadillac CT4-V And CT5-V Have Landed, But They're Not That Powerful</t>
+  </si>
+  <si>
+    <t>The Cadillac CT5 Is Here To Replace The ATS And CTS</t>
+  </si>
+  <si>
+    <t>The Jaguar XE SV Project 8 Is Now Laguna Seca's Fastest Saloon</t>
+  </si>
+  <si>
+    <t>SUVs Are Now 46 Times More Popular Than Sports Cars</t>
+  </si>
+  <si>
+    <t>The Euro NCAP Zero-Star Fiat Punto Has Been Axed</t>
+  </si>
+  <si>
+    <t>The 808bhp V12 Hybrid Sian Is Lamborghini's Fastest Car Ever</t>
+  </si>
+  <si>
+    <t>Say Hello To Albert: The 250mph McLaren Speedtail Prototype</t>
+  </si>
+  <si>
+    <t>The Lancia Delta Futurista Is A €300k 'Reimagined' Integrale</t>
+  </si>
+  <si>
+    <t>A £2.5 Million Porsche 959 Dakar Is For Sale For The First Time Ever</t>
+  </si>
+  <si>
+    <t>The Infiniti Brand Will Soon Be Dead In Europe</t>
+  </si>
+  <si>
+    <t>Cupra's First Self-Designed Car Is A Lowered SUV With A Coupe Roof Line</t>
+  </si>
+  <si>
+    <t>A 370Z Replacement Is Being Worked On, Senior Nissan Figure Confirms</t>
+  </si>
+  <si>
+    <t>Brace For The Weirdness Of Hyundai's Kona 'Iron Man Edition'</t>
+  </si>
+  <si>
+    <t>Nissan Has Started Production Of Brand New R33 And R34 Skyline GT-R Parts</t>
+  </si>
+  <si>
+    <t>Toyota Is Putting A80 Supra Components Back Into Production</t>
+  </si>
+  <si>
+    <t>The New Vauxhall Corsa Is Coming With Its Electric Powertrain And Fancy Lights</t>
+  </si>
+  <si>
+    <t>McLaren Is Building A New Mid-Engined Grand Tourer</t>
+  </si>
+  <si>
+    <t>The Regular Vauxhall Corsa Is Here, And It Weighs Just 980kg</t>
+  </si>
+  <si>
+    <t>The First Ever Fully Electric Vauxhall Corsa Is Here With A 205-Mile Range</t>
+  </si>
+  <si>
+    <t>McLaren Is Making An Ultimate Series Car With No Windscreen</t>
+  </si>
+  <si>
+    <t>Koenigsegg’s New Jesko Is A £2.3 Million Route To 1578bhp</t>
+  </si>
+  <si>
+    <t>Hennessey Is Targetting 500kmh With The Venom F5</t>
+  </si>
+  <si>
+    <t>300mph Will Be A 'Baseline' For The Hennessey Venom F5</t>
+  </si>
+  <si>
+    <t>The SSC Tuatara Is Coming Back With A Top Speed Over 278mph</t>
+  </si>
+  <si>
+    <t>Bugatti’s ‘La Voiture Noire’ GT Is The Most Expensive Road Car Ever</t>
+  </si>
+  <si>
+    <t>The Rimac-Powered Pininfarina Battista Shocks Geneva With 1877bhp</t>
+  </si>
+  <si>
+    <t>The Chiron Sport ‘110 Ans Bugatti' Is A 1500bhp French-Themed Tribute</t>
+  </si>
+  <si>
+    <t>The Bugatti Centodieci Is A Chiron In An EB110-Like Frock</t>
+  </si>
+  <si>
+    <t>Pininfarina Has Secured Rimac Power For The 1900bhp PF0 Hypercar</t>
+  </si>
+  <si>
+    <t>Pininfarina's New Electric Hypercar Nearly Here, Will Do 0-62 In Under 2sec</t>
+  </si>
+  <si>
+    <t>A Pininfarina-Designed Karma EV Is On The Way</t>
+  </si>
+  <si>
+    <t>Lamborghini’s 631bhp Huracan Evo Has Spawned A Soft-Top Spyder</t>
+  </si>
+  <si>
+    <t>A Bugatti SUV Is Definitely Not Happening, Says CEO</t>
+  </si>
+  <si>
+    <t>The New Audi S8 Has A 563bhp Mild Hybrid Petrol V8</t>
+  </si>
+  <si>
+    <t>The Bentley Bentayga Speed Is Here And It'll Do 190mph</t>
+  </si>
+  <si>
+    <t>There's A 2.0-Litre Toyota Supra And It Could Replace The GT86</t>
+  </si>
+  <si>
+    <t>Toyota Wants To Revive The MR2, And It Might End Up Being Electric</t>
   </si>
 </sst>
 </file>
@@ -350,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A3"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -373,6 +631,441 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>